<commit_message>
added to descriptives, cleaned psm
</commit_message>
<xml_diff>
--- a/04_results/baltest_bygroup_pre.xlsx
+++ b/04_results/baltest_bygroup_pre.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="65">
   <si>
     <t/>
   </si>
@@ -21,6 +21,15 @@
     <t>Variable</t>
   </si>
   <si>
+    <t>OWN</t>
+  </si>
+  <si>
+    <t>TECH</t>
+  </si>
+  <si>
+    <t>PORT</t>
+  </si>
+  <si>
     <t>logwages2015</t>
   </si>
   <si>
@@ -60,6 +69,24 @@
     <t>Mean/SE</t>
   </si>
   <si>
+    <t>2.814</t>
+  </si>
+  <si>
+    <t>[0.011]</t>
+  </si>
+  <si>
+    <t>2.565</t>
+  </si>
+  <si>
+    <t>[0.014]</t>
+  </si>
+  <si>
+    <t>0.273</t>
+  </si>
+  <si>
+    <t>[0.005]</t>
+  </si>
+  <si>
     <t>7.529</t>
   </si>
   <si>
@@ -102,6 +129,24 @@
     <t>1</t>
   </si>
   <si>
+    <t>3.004</t>
+  </si>
+  <si>
+    <t>[0.012]</t>
+  </si>
+  <si>
+    <t>1.838</t>
+  </si>
+  <si>
+    <t>[0.015]</t>
+  </si>
+  <si>
+    <t>0.467</t>
+  </si>
+  <si>
+    <t>[0.007]</t>
+  </si>
+  <si>
     <t>7.031</t>
   </si>
   <si>
@@ -123,9 +168,6 @@
     <t>0.493</t>
   </si>
   <si>
-    <t>[0.005]</t>
-  </si>
-  <si>
     <t>0.204</t>
   </si>
   <si>
@@ -139,6 +181,15 @@
   </si>
   <si>
     <t>(1)-(2)</t>
+  </si>
+  <si>
+    <t>-0.191***</t>
+  </si>
+  <si>
+    <t>0.728***</t>
+  </si>
+  <si>
+    <t>-0.194***</t>
   </si>
   <si>
     <t>0.498***</t>
@@ -200,7 +251,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F23"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -211,16 +262,16 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>27</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>39</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2">
@@ -231,16 +282,16 @@
         <v>0</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="D2" t="s">
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3">
@@ -248,19 +299,19 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="F3" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4">
@@ -268,19 +319,19 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E4" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="F4" t="s">
-        <v>42</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5">
@@ -291,13 +342,13 @@
         <v>0</v>
       </c>
       <c r="C5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D5" t="s">
         <v>0</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
         <v>0</v>
@@ -308,19 +359,19 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E6" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="F6" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
@@ -331,13 +382,13 @@
         <v>0</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="D7" t="s">
         <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>32</v>
+        <v>41</v>
       </c>
       <c r="F7" t="s">
         <v>0</v>
@@ -348,19 +399,19 @@
         <v>4</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E8" t="s">
-        <v>33</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>44</v>
+        <v>58</v>
       </c>
     </row>
     <row r="9">
@@ -371,13 +422,13 @@
         <v>0</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
         <v>0</v>
       </c>
       <c r="E9" t="s">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
         <v>0</v>
@@ -388,19 +439,19 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E10" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="F10" t="s">
-        <v>45</v>
+        <v>59</v>
       </c>
     </row>
     <row r="11">
@@ -411,13 +462,13 @@
         <v>0</v>
       </c>
       <c r="C11" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D11" t="s">
         <v>0</v>
       </c>
       <c r="E11" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="F11" t="s">
         <v>0</v>
@@ -428,19 +479,19 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C12" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="D12" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E12" t="s">
-        <v>37</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
-        <v>46</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13">
@@ -451,13 +502,13 @@
         <v>0</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>24</v>
+        <v>47</v>
       </c>
       <c r="F13" t="s">
         <v>0</v>
@@ -468,19 +519,19 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="D14" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="E14" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="F14" t="s">
-        <v>47</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15">
@@ -491,13 +542,13 @@
         <v>0</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
       <c r="D15" t="s">
         <v>0</v>
       </c>
       <c r="E15" t="s">
-        <v>36</v>
+        <v>49</v>
       </c>
       <c r="F15" t="s">
         <v>0</v>
@@ -508,38 +559,158 @@
         <v>8</v>
       </c>
       <c r="B16" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>0</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E16" t="s">
-        <v>0</v>
+        <v>50</v>
       </c>
       <c r="F16" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" t="s">
+        <v>23</v>
+      </c>
+      <c r="F17" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
         <v>9</v>
       </c>
-      <c r="B17" t="s">
-        <v>0</v>
-      </c>
-      <c r="C17" t="s">
-        <v>0</v>
-      </c>
-      <c r="D17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E17" t="s">
-        <v>0</v>
-      </c>
-      <c r="F17" t="s">
+      <c r="B18" t="s">
+        <v>14</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E18" t="s">
+        <v>51</v>
+      </c>
+      <c r="F18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>0</v>
+      </c>
+      <c r="E19" t="s">
+        <v>33</v>
+      </c>
+      <c r="F19" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" t="s">
+        <v>52</v>
+      </c>
+      <c r="F20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" t="s">
+        <v>31</v>
+      </c>
+      <c r="D21" t="s">
+        <v>0</v>
+      </c>
+      <c r="E21" t="s">
+        <v>23</v>
+      </c>
+      <c r="F21" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B22" t="s">
+        <v>0</v>
+      </c>
+      <c r="C22" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+      <c r="C23" t="s">
+        <v>0</v>
+      </c>
+      <c r="D23" t="s">
+        <v>0</v>
+      </c>
+      <c r="E23" t="s">
+        <v>0</v>
+      </c>
+      <c r="F23" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>